<commit_message>
qaqc scripts for path 3A and 3B
</commit_message>
<xml_diff>
--- a/path_3b/data/01_raw/data_contributor_3/dataset3.xlsx
+++ b/path_3b/data/01_raw/data_contributor_3/dataset3.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2558" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2561" uniqueCount="236">
   <si>
     <t>Chromis acares</t>
   </si>
@@ -1052,10 +1052,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H774"/>
+  <dimension ref="A1:H775"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A737" workbookViewId="0">
-      <selection activeCell="F759" sqref="F759"/>
+    <sheetView tabSelected="1" topLeftCell="A755" workbookViewId="0">
+      <selection activeCell="G776" sqref="G776"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21181,6 +21181,32 @@
         <v>1</v>
       </c>
       <c r="H774">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="775" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A775">
+        <v>2016</v>
+      </c>
+      <c r="B775" s="1">
+        <v>42514</v>
+      </c>
+      <c r="C775" t="s">
+        <v>116</v>
+      </c>
+      <c r="D775" t="s">
+        <v>235</v>
+      </c>
+      <c r="E775">
+        <v>1</v>
+      </c>
+      <c r="F775" t="s">
+        <v>234</v>
+      </c>
+      <c r="G775">
+        <v>-15</v>
+      </c>
+      <c r="H775">
         <v>5</v>
       </c>
     </row>

</xml_diff>